<commit_message>
sort codes after getting new am_tram_stations
</commit_message>
<xml_diff>
--- a/notebooks/am_tram_stations.xlsx
+++ b/notebooks/am_tram_stations.xlsx
@@ -8726,12 +8726,12 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
           <t>Centraal Station_B</t>
-        </is>
-      </c>
-      <c r="D213" t="inlineStr">
-        <is>
-          <t>Centraal Station</t>
         </is>
       </c>
       <c r="E213" t="inlineStr"/>
@@ -8765,12 +8765,12 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
           <t>Centraal Station_A</t>
-        </is>
-      </c>
-      <c r="D214" t="inlineStr">
-        <is>
-          <t>Centraal Station</t>
         </is>
       </c>
       <c r="E214" t="inlineStr"/>

</xml_diff>